<commit_message>
new test employee leave
</commit_message>
<xml_diff>
--- a/src/test/resources/EmployeeDetails.xlsx
+++ b/src/test/resources/EmployeeDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Orangehrm\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A6CF9E-67E9-4F7C-B465-6E4A82CAB6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F75234-060A-43C5-B2AF-34247A61F762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>Chirag#1234</t>
   </si>
   <si>
-    <t>rai</t>
-  </si>
-  <si>
     <t>First Name</t>
   </si>
   <si>
@@ -58,6 +55,9 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>Rai</t>
   </si>
 </sst>
 </file>
@@ -377,8 +377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -388,7 +388,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -396,7 +396,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -404,15 +404,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>1012</v>
@@ -420,7 +420,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -428,7 +428,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -436,7 +436,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>

</xml_diff>